<commit_message>
Surface Water Data: fix formatting issues
-Reformat all data to be consistent in coluumns.
-Add pivot tables.
-Delete dupicate graph.
-Remove unused sheet.
</commit_message>
<xml_diff>
--- a/CW 1 Assignment II Surface Water Data(1).xlsx
+++ b/CW 1 Assignment II Surface Water Data(1).xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lockh\Documents\University\Environmental Engineering\Hydrology and Hydrogeology\Coursework 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\dlim\Documents\surface_water_data_manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ADA28F-951B-40E8-BC54-71EF86CC6A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907DD47F-40E6-47E0-8ABB-EDFEB0BB8AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5235" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dilution" sheetId="4" r:id="rId1"/>
     <sheet name="Rating" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -113,9 +112,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -164,11 +164,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -643,7 +672,7 @@
             <c:numRef>
               <c:f>Dilution!$B$8:$B$128</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="121"/>
                 <c:pt idx="0">
                   <c:v>206.3</c:v>
@@ -1112,7 +1141,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1220,1030 +1249,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Dilution!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Specific Conductance (uS/cm)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Dilution!$A$8:$A$128</c:f>
-              <c:numCache>
-                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="121"/>
-                <c:pt idx="0">
-                  <c:v>44503.466840277775</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44503.466863425929</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44503.466874999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44503.466886574075</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44503.466898148145</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44503.466909722221</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44503.466921296298</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44503.466932870368</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44503.466944444444</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44503.466956018521</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44503.466967592591</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44503.466979166667</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44503.466990740744</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44503.467002314814</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44503.467013888891</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44503.46702546296</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44503.467037037037</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44503.467048611114</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44503.467060185183</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44503.46707175926</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44503.467083333337</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44503.467094907406</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44503.467106481483</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44503.467118055552</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44503.467129629629</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44503.467141203706</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44503.467152777775</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44503.467164351852</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44503.467175925929</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44503.467187499999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44503.467199074075</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44503.467210648145</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44503.467222222222</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44503.467233796298</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44503.467245370368</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44503.467256944445</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44503.467268518521</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44503.467280092591</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44503.467291666668</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44503.467303240737</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>44503.467314814814</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>44503.467326388891</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>44503.46733796296</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44503.467349537037</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44503.467361111114</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>44503.467372685183</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44503.46738425926</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>44503.467395833337</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>44503.467407407406</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>44503.467418981483</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>44503.467430555553</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>44503.467442129629</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>44503.467453703706</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>44503.467465277776</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>44503.467476851853</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>44503.467488425929</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>44503.467499999999</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>44503.467511574076</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>44503.467523148145</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>44503.467534722222</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>44503.467546296299</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>44503.467557870368</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>44503.467569444445</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>44503.467581018522</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>44503.467592592591</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>44503.467604166668</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>44503.467615740738</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>44503.467627314814</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>44503.467638888891</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>44503.467650462961</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>44503.467662037037</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>44503.467673611114</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>44503.467685185184</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>44503.46769675926</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>44503.46770833333</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>44503.467719907407</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>44503.467731481483</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>44503.467743055553</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>44503.46775462963</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>44503.467766203707</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>44503.467777777776</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>44503.467789351853</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>44503.467800925922</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>44503.467812499999</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>44503.467824074076</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>44503.467835648145</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>44503.467847222222</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>44503.467858796299</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>44503.467870370368</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>44503.467881944445</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>44503.467893518522</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>44503.467905092592</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>44503.467916666668</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>44503.467928240738</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>44503.467939814815</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>44503.467951388891</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>44503.467962962961</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>44503.467974537038</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>44503.467986111114</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>44503.467997685184</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>44503.468009259261</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>44503.46802083333</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>44503.468032407407</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>44503.468043981484</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>44503.468055555553</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>44503.46806712963</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>44503.468078703707</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>44503.468090277776</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>44503.468101851853</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>44503.468113425923</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>44503.468124999999</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>44503.468136574076</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>44503.468148148146</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>44503.468159722222</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>44503.468171296299</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>44503.468182870369</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>44503.468194444446</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>44503.468206018515</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>44503.468217592592</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>44503.468229166669</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>44503.468240740738</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Dilution!$B$8:$B$128</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="121"/>
-                <c:pt idx="0">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>234.6</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>297.2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>328.5</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>354</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>328.9</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>316.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>290.2</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>268.10000000000002</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>250.2</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>241.3</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>232.9</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>227.1</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>224.2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>217.8</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>216.3</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>214.8</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>213.5</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>212.4</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>211.8</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>211.2</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>210.6</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>210.3</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>209.8</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>209.2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>208.9</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>208.7</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>208.2</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>207.5</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>207.1</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>207.3</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>207.2</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>207.2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>207.1</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>206.9</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>206.8</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>206.7</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>206.4</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>206.5</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>206.4</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>206.3</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>206.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E31B-4EA9-918C-787438B3EA88}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1417933519"/>
-        <c:axId val="1417934959"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1417933519"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1417934959"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1417934959"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1417933519"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2392,7 +1397,7 @@
             <c:numRef>
               <c:f>Rating!$A$6:$A$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.9999999999999997E-2</c:v>
@@ -2598,7 +1603,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2930,46 +1935,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4002,536 +2967,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>61852</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28285</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>525677</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185656</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>503464</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>576</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>354376</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>157947</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4551,42 +3000,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>496956</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>77857</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>165652</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>154057</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82D89970-34A8-CF5D-29E7-DCCB33D9D431}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4634,6 +3047,34 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B57CF595-A9D4-475E-BBE7-842F05F59C43}" name="Table1" displayName="Table1" ref="A7:D128" totalsRowShown="0">
+  <autoFilter ref="A7:D128" xr:uid="{B57CF595-A9D4-475E-BBE7-842F05F59C43}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{483B9437-FD6A-4F56-B7DE-77FD0F94D1F2}" name="Time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7AA644D5-67F2-44A6-8708-9BFEE5347F6C}" name="Specific Conductance (uS/cm)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8A3CE483-A7B1-41BB-9350-B3E89CEA576B}" name="C2-C0" dataDxfId="3">
+      <calculatedColumnFormula>B8-$F$4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{158F9E36-E1C4-40B5-BC34-8E4EFEE51619}" name="(C2-C0) dt" dataDxfId="2">
+      <calculatedColumnFormula>C8</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{17F5D3A8-FA20-4374-98F8-E7086FF604C0}" name="Table2" displayName="Table2" ref="A5:B20" totalsRowShown="0">
+  <autoFilter ref="A5:B20" xr:uid="{17F5D3A8-FA20-4374-98F8-E7086FF604C0}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{59802D42-A7A5-49FC-B2BD-C6E8899DB265}" name="Stage (m)" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B679B0E7-C12C-44B5-A678-3437C6C35437}" name="Discharge (m3/sec)" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4901,14 +3342,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -4986,1937 +3428,1937 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="8">
         <v>44503.466840277775</v>
       </c>
-      <c r="B8" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C8" s="6">
         <f>B8-$F$4</f>
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <f>C8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="8">
         <v>44503.466863425929</v>
       </c>
-      <c r="B9" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C9" s="6">
         <f>B9-$F$4</f>
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <f t="shared" ref="D9:D72" si="0">C9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <v>44503.466874999998</v>
       </c>
-      <c r="B10" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C10" s="6">
         <f t="shared" ref="C10:C72" si="1">B10-$F$4</f>
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="8">
         <v>44503.466886574075</v>
       </c>
-      <c r="B11" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="8">
         <v>44503.466898148145</v>
       </c>
-      <c r="B12" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="8">
         <v>44503.466909722221</v>
       </c>
-      <c r="B13" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="8">
         <v>44503.466921296298</v>
       </c>
-      <c r="B14" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="8">
         <v>44503.466932870368</v>
       </c>
-      <c r="B15" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="8">
         <v>44503.466944444444</v>
       </c>
-      <c r="B16" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="8">
         <v>44503.466956018521</v>
       </c>
-      <c r="B17" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="8">
         <v>44503.466967592591</v>
       </c>
-      <c r="B18" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="8">
         <v>44503.466979166667</v>
       </c>
-      <c r="B19" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="8">
         <v>44503.466990740744</v>
       </c>
-      <c r="B20" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="8">
         <v>44503.467002314814</v>
       </c>
-      <c r="B21" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="8">
         <v>44503.467013888891</v>
       </c>
-      <c r="B22" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="8">
         <v>44503.46702546296</v>
       </c>
-      <c r="B23" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="8">
         <v>44503.467037037037</v>
       </c>
-      <c r="B24" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24">
+      <c r="B24" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="8">
         <v>44503.467048611114</v>
       </c>
-      <c r="B25" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="B25" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="8">
         <v>44503.467060185183</v>
       </c>
-      <c r="B26" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="8">
         <v>44503.46707175926</v>
       </c>
-      <c r="B27" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D27">
+      <c r="B27" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="8">
         <v>44503.467083333337</v>
       </c>
-      <c r="B28" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D28">
+      <c r="B28" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="8">
         <v>44503.467094907406</v>
       </c>
-      <c r="B29" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D29">
+      <c r="B29" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="8">
         <v>44503.467106481483</v>
       </c>
-      <c r="B30" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D30">
+      <c r="B30" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="8">
         <v>44503.467118055552</v>
       </c>
-      <c r="B31" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="8">
         <v>44503.467129629629</v>
       </c>
-      <c r="B32" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D32">
+      <c r="B32" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="8">
         <v>44503.467141203706</v>
       </c>
-      <c r="B33" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D33">
+      <c r="B33" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="8">
         <v>44503.467152777775</v>
       </c>
-      <c r="B34" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="B34" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="8">
         <v>44503.467164351852</v>
       </c>
-      <c r="B35" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D35">
+      <c r="B35" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="8">
         <v>44503.467175925929</v>
       </c>
-      <c r="B36" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D36">
+      <c r="B36" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="8">
         <v>44503.467187499999</v>
       </c>
-      <c r="B37" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D37">
+      <c r="B37" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="8">
         <v>44503.467199074075</v>
       </c>
-      <c r="B38" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D38">
+      <c r="B38" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="8">
         <v>44503.467210648145</v>
       </c>
-      <c r="B39" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="8">
         <v>44503.467222222222</v>
       </c>
-      <c r="B40" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D40">
+      <c r="B40" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="8">
         <v>44503.467233796298</v>
       </c>
-      <c r="B41" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D41">
+      <c r="B41" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="8">
         <v>44503.467245370368</v>
       </c>
-      <c r="B42" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D42">
+      <c r="B42" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="8">
         <v>44503.467256944445</v>
       </c>
-      <c r="B43" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D43">
+      <c r="B43" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="8">
         <v>44503.467268518521</v>
       </c>
-      <c r="B44" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D44">
+      <c r="B44" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="8">
         <v>44503.467280092591</v>
       </c>
-      <c r="B45" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D45">
+      <c r="B45" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="8">
         <v>44503.467291666668</v>
       </c>
-      <c r="B46" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D46">
+      <c r="B46" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="8">
         <v>44503.467303240737</v>
       </c>
-      <c r="B47" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D47">
+      <c r="B47" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="8">
         <v>44503.467314814814</v>
       </c>
-      <c r="B48" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D48">
+      <c r="B48" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="8">
         <v>44503.467326388891</v>
       </c>
-      <c r="B49" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D49">
+      <c r="B49" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="8">
         <v>44503.46733796296</v>
       </c>
-      <c r="B50" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D50">
+      <c r="B50" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="8">
         <v>44503.467349537037</v>
       </c>
-      <c r="B51" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D51">
+      <c r="B51" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="8">
         <v>44503.467361111114</v>
       </c>
-      <c r="B52" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D52">
+      <c r="B52" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="8">
         <v>44503.467372685183</v>
       </c>
-      <c r="B53" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D53">
+      <c r="B53" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C53" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="8">
         <v>44503.46738425926</v>
       </c>
-      <c r="B54" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D54">
+      <c r="B54" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="8">
         <v>44503.467395833337</v>
       </c>
-      <c r="B55" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D55">
+      <c r="B55" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="8">
         <v>44503.467407407406</v>
       </c>
-      <c r="B56" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D56">
+      <c r="B56" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D56" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="8">
         <v>44503.467418981483</v>
       </c>
-      <c r="B57" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C57">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D57">
+      <c r="B57" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C57" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D57" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="8">
         <v>44503.467430555553</v>
       </c>
-      <c r="B58" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D58">
+      <c r="B58" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C58" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D58" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="8">
         <v>44503.467442129629</v>
       </c>
-      <c r="B59" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D59">
+      <c r="B59" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="8">
         <v>44503.467453703706</v>
       </c>
-      <c r="B60" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D60">
+      <c r="B60" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C60" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D60" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="8">
         <v>44503.467465277776</v>
       </c>
-      <c r="B61" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D61">
+      <c r="B61" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C61" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="8">
         <v>44503.467476851853</v>
       </c>
-      <c r="B62" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D62">
+      <c r="B62" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C62" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="8">
         <v>44503.467488425929</v>
       </c>
-      <c r="B63" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D63">
+      <c r="B63" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C63" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D63" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="8">
         <v>44503.467499999999</v>
       </c>
-      <c r="B64" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C64">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D64">
+      <c r="B64" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C64" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D64" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="8">
         <v>44503.467511574076</v>
       </c>
-      <c r="B65" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D65">
+      <c r="B65" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C65" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D65" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="8">
         <v>44503.467523148145</v>
       </c>
-      <c r="B66" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D66">
+      <c r="B66" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C66" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D66" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="8">
         <v>44503.467534722222</v>
       </c>
-      <c r="B67" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D67">
+      <c r="B67" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C67" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D67" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="8">
         <v>44503.467546296299</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="7">
         <v>234.6</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="6">
         <f t="shared" si="1"/>
         <v>28.299999999999983</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="6">
         <f t="shared" si="0"/>
         <v>28.299999999999983</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="8">
         <v>44503.467557870368</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="7">
         <v>297.2</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="6">
         <f t="shared" si="1"/>
         <v>90.899999999999977</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="6">
         <f t="shared" si="0"/>
         <v>90.899999999999977</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="8">
         <v>44503.467569444445</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="7">
         <v>328.5</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="6">
         <f t="shared" si="1"/>
         <v>122.19999999999999</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="6">
         <f t="shared" si="0"/>
         <v>122.19999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="8">
         <v>44503.467581018522</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="7">
         <v>354</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="6">
         <f t="shared" si="1"/>
         <v>147.69999999999999</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="6">
         <f t="shared" si="0"/>
         <v>147.69999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="8">
         <v>44503.467592592591</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="7">
         <v>328.9</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="6">
         <f t="shared" si="1"/>
         <v>122.59999999999997</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="6">
         <f t="shared" si="0"/>
         <v>122.59999999999997</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="8">
         <v>44503.467604166668</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="7">
         <v>316.39999999999998</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="6">
         <f t="shared" ref="C73:C128" si="2">B73-$F$4</f>
         <v>110.09999999999997</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="6">
         <f t="shared" ref="D73:D128" si="3">C73</f>
         <v>110.09999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="8">
         <v>44503.467615740738</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="7">
         <v>290.2</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="6">
         <f t="shared" si="2"/>
         <v>83.899999999999977</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="6">
         <f t="shared" si="3"/>
         <v>83.899999999999977</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="8">
         <v>44503.467627314814</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="7">
         <v>268.10000000000002</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="6">
         <f t="shared" si="2"/>
         <v>61.800000000000011</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="6">
         <f t="shared" si="3"/>
         <v>61.800000000000011</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="8">
         <v>44503.467638888891</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="7">
         <v>250.2</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="6">
         <f t="shared" si="2"/>
         <v>43.899999999999977</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="6">
         <f t="shared" si="3"/>
         <v>43.899999999999977</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="8">
         <v>44503.467650462961</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="7">
         <v>241.3</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="6">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="6">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="8">
         <v>44503.467662037037</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="7">
         <v>232.9</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="6">
         <f t="shared" si="2"/>
         <v>26.599999999999994</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="6">
         <f t="shared" si="3"/>
         <v>26.599999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="8">
         <v>44503.467673611114</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="7">
         <v>227.1</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="6">
         <f t="shared" si="2"/>
         <v>20.799999999999983</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="6">
         <f t="shared" si="3"/>
         <v>20.799999999999983</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="8">
         <v>44503.467685185184</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="7">
         <v>224.2</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="6">
         <f t="shared" si="2"/>
         <v>17.899999999999977</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="6">
         <f t="shared" si="3"/>
         <v>17.899999999999977</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="8">
         <v>44503.46769675926</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="7">
         <v>221</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="6">
         <f t="shared" si="2"/>
         <v>14.699999999999989</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="6">
         <f t="shared" si="3"/>
         <v>14.699999999999989</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="8">
         <v>44503.46770833333</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="7">
         <v>217.8</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="6">
         <f t="shared" si="2"/>
         <v>11.5</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="6">
         <f t="shared" si="3"/>
         <v>11.5</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="8">
         <v>44503.467719907407</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="7">
         <v>216.3</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="6">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="8">
         <v>44503.467731481483</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="7">
         <v>214.8</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="6">
         <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="6">
         <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="8">
         <v>44503.467743055553</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="7">
         <v>213.5</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="6">
         <f t="shared" si="2"/>
         <v>7.1999999999999886</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="6">
         <f t="shared" si="3"/>
         <v>7.1999999999999886</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="8">
         <v>44503.46775462963</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="7">
         <v>212.4</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="6">
         <f t="shared" si="2"/>
         <v>6.0999999999999943</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="6">
         <f t="shared" si="3"/>
         <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="8">
         <v>44503.467766203707</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="7">
         <v>211.8</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="6">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="6">
         <f t="shared" si="3"/>
         <v>5.5</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="8">
         <v>44503.467777777776</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="7">
         <v>211.2</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="6">
         <f t="shared" si="2"/>
         <v>4.8999999999999773</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="6">
         <f t="shared" si="3"/>
         <v>4.8999999999999773</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="8">
         <v>44503.467789351853</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="7">
         <v>210.6</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="6">
         <f t="shared" si="2"/>
         <v>4.2999999999999829</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="6">
         <f t="shared" si="3"/>
         <v>4.2999999999999829</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="8">
         <v>44503.467800925922</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="7">
         <v>210.3</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="8">
         <v>44503.467812499999</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="7">
         <v>209.8</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="6">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="6">
         <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="8">
         <v>44503.467824074076</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="7">
         <v>209.2</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="6">
         <f t="shared" si="2"/>
         <v>2.8999999999999773</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="6">
         <f t="shared" si="3"/>
         <v>2.8999999999999773</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="8">
         <v>44503.467835648145</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="7">
         <v>208.9</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="6">
         <f t="shared" si="2"/>
         <v>2.5999999999999943</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="6">
         <f t="shared" si="3"/>
         <v>2.5999999999999943</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="8">
         <v>44503.467847222222</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="7">
         <v>208.7</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="6">
         <f t="shared" si="2"/>
         <v>2.3999999999999773</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="6">
         <f t="shared" si="3"/>
         <v>2.3999999999999773</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="8">
         <v>44503.467858796299</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="7">
         <v>208.2</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="6">
         <f t="shared" si="2"/>
         <v>1.8999999999999773</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="6">
         <f t="shared" si="3"/>
         <v>1.8999999999999773</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="8">
         <v>44503.467870370368</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="7">
         <v>207.5</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="6">
         <f t="shared" si="2"/>
         <v>1.1999999999999886</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="6">
         <f t="shared" si="3"/>
         <v>1.1999999999999886</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="8">
         <v>44503.467881944445</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="7">
         <v>207.1</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="6">
         <f t="shared" si="2"/>
         <v>0.79999999999998295</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="6">
         <f t="shared" si="3"/>
         <v>0.79999999999998295</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="8">
         <v>44503.467893518522</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="7">
         <v>207.3</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="8">
         <v>44503.467905092592</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="7">
         <v>207.2</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="6">
         <f t="shared" si="2"/>
         <v>0.89999999999997726</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="6">
         <f t="shared" si="3"/>
         <v>0.89999999999997726</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="8">
         <v>44503.467916666668</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="7">
         <v>207.2</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="6">
         <f t="shared" si="2"/>
         <v>0.89999999999997726</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="6">
         <f t="shared" si="3"/>
         <v>0.89999999999997726</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="8">
         <v>44503.467928240738</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="7">
         <v>207.1</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="6">
         <f t="shared" si="2"/>
         <v>0.79999999999998295</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="6">
         <f t="shared" si="3"/>
         <v>0.79999999999998295</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="8">
         <v>44503.467939814815</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="7">
         <v>206.9</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="6">
         <f t="shared" si="2"/>
         <v>0.59999999999999432</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="6">
         <f t="shared" si="3"/>
         <v>0.59999999999999432</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="8">
         <v>44503.467951388891</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="7">
         <v>206.8</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="8">
         <v>44503.467962962961</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="7">
         <v>206.8</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="8">
         <v>44503.467974537038</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="7">
         <v>206.8</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="8">
         <v>44503.467986111114</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="7">
         <v>206.7</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="8">
         <v>44503.467997685184</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="7">
         <v>206.7</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="8">
         <v>44503.468009259261</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="7">
         <v>206.8</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="8">
         <v>44503.46802083333</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="7">
         <v>206.8</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="8">
         <v>44503.468032407407</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110" s="7">
         <v>206.8</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="6">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="8">
         <v>44503.468043981484</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="7">
         <v>206.7</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="8">
         <v>44503.468055555553</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="7">
         <v>206.7</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="8">
         <v>44503.46806712963</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="7">
         <v>206.7</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="8">
         <v>44503.468078703707</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="7">
         <v>206.7</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="6">
         <f t="shared" si="2"/>
         <v>0.39999999999997726</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="6">
         <f t="shared" si="3"/>
         <v>0.39999999999997726</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="8">
         <v>44503.468090277776</v>
       </c>
-      <c r="B115" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C115">
+      <c r="B115" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C115" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="8">
         <v>44503.468101851853</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B116" s="7">
         <v>206.4</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="6">
         <f t="shared" si="2"/>
         <v>9.9999999999994316E-2</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="6">
         <f t="shared" si="3"/>
         <v>9.9999999999994316E-2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="8">
         <v>44503.468113425923</v>
       </c>
-      <c r="B117" s="3">
+      <c r="B117" s="7">
         <v>206.5</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="6">
         <f t="shared" si="2"/>
         <v>0.19999999999998863</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="6">
         <f t="shared" si="3"/>
         <v>0.19999999999998863</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="8">
         <v>44503.468124999999</v>
       </c>
-      <c r="B118" s="3">
+      <c r="B118" s="7">
         <v>206.4</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="6">
         <f t="shared" si="2"/>
         <v>9.9999999999994316E-2</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="6">
         <f t="shared" si="3"/>
         <v>9.9999999999994316E-2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="8">
         <v>44503.468136574076</v>
       </c>
-      <c r="B119" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C119">
+      <c r="B119" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C119" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="8">
         <v>44503.468148148146</v>
       </c>
-      <c r="B120" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C120">
+      <c r="B120" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C120" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="8">
         <v>44503.468159722222</v>
       </c>
-      <c r="B121" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C121">
+      <c r="B121" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C121" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="8">
         <v>44503.468171296299</v>
       </c>
-      <c r="B122" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C122">
+      <c r="B122" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C122" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="8">
         <v>44503.468182870369</v>
       </c>
-      <c r="B123" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C123">
+      <c r="B123" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C123" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="8">
         <v>44503.468194444446</v>
       </c>
-      <c r="B124" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C124">
+      <c r="B124" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C124" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="8">
         <v>44503.468206018515</v>
       </c>
-      <c r="B125" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C125">
+      <c r="B125" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C125" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="8">
         <v>44503.468217592592</v>
       </c>
-      <c r="B126" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C126">
+      <c r="B126" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C126" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="8">
         <v>44503.468229166669</v>
       </c>
-      <c r="B127" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C127">
+      <c r="B127" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C127" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="8">
         <v>44503.468240740738</v>
       </c>
-      <c r="B128" s="3">
-        <v>206.3</v>
-      </c>
-      <c r="C128">
+      <c r="B128" s="7">
+        <v>206.3</v>
+      </c>
+      <c r="C128" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6924,6 +5366,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6931,14 +5376,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6965,7 +5410,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>1.9999999999999997E-2</v>
       </c>
       <c r="B6" s="4">
@@ -6973,7 +5418,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>0.03</v>
       </c>
       <c r="B7" s="4">
@@ -6981,7 +5426,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>0.04</v>
       </c>
       <c r="B8" s="4">
@@ -6989,7 +5434,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>0.05</v>
       </c>
       <c r="B9" s="4">
@@ -6997,7 +5442,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="5">
         <v>0.1</v>
       </c>
       <c r="B10" s="4">
@@ -7005,12 +5450,12 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>0.2</v>
       </c>
       <c r="B12" s="4">
@@ -7018,7 +5463,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>0.25</v>
       </c>
       <c r="B13" s="4">
@@ -7026,7 +5471,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>0.3</v>
       </c>
       <c r="B14" s="4">
@@ -7034,7 +5479,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>0.35</v>
       </c>
       <c r="B15" s="4">
@@ -7042,7 +5487,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="5">
         <v>0.39999999999999997</v>
       </c>
       <c r="B16" s="4">
@@ -7050,7 +5495,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>0.44999999999999996</v>
       </c>
       <c r="B17" s="4">
@@ -7058,7 +5503,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="5">
         <v>0.49999999999999994</v>
       </c>
       <c r="B18" s="4">
@@ -7066,7 +5511,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>0.54999999999999993</v>
       </c>
       <c r="B19" s="4">
@@ -7074,7 +5519,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>0.6</v>
       </c>
       <c r="B20" s="4">
@@ -7107,41 +5552,13 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B0B185-160A-48B7-AEDF-76D348659D3F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4a7669a9-a011-4939-9a62-ac1a8914829f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006406AF6E899A443B088CBB235517035" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="386f34c9231fac88c8ace8375b5a25b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4a7669a9-a011-4939-9a62-ac1a8914829f" xmlns:ns4="c51ce0d9-b5e0-4520-89e9-ff5f84fa91bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05a26a0affa2f84da2894de9713acc90" ns3:_="" ns4:_="">
     <xsd:import namespace="4a7669a9-a011-4939-9a62-ac1a8914829f"/>
@@ -7394,10 +5811,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4a7669a9-a011-4939-9a62-ac1a8914829f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D169B7-BC98-4638-8EC9-DE9AE9B79DD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31EB3A26-3559-44C0-8F16-CE56C6070923}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4a7669a9-a011-4939-9a62-ac1a8914829f"/>
+    <ds:schemaRef ds:uri="c51ce0d9-b5e0-4520-89e9-ff5f84fa91bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7420,20 +5865,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31EB3A26-3559-44C0-8F16-CE56C6070923}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D169B7-BC98-4638-8EC9-DE9AE9B79DD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4a7669a9-a011-4939-9a62-ac1a8914829f"/>
-    <ds:schemaRef ds:uri="c51ce0d9-b5e0-4520-89e9-ff5f84fa91bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>